<commit_message>
created most of the results, cleaned up, generated all the data
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mokronos\code\nonlinearLSTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACEC630-2A5C-4769-AEB2-D2C987E2F383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DCAC21-35F8-4A56-BF31-C7CBE713FC12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10500" yWindow="4860" windowWidth="21600" windowHeight="11385" xr2:uid="{54E0EE64-5DA5-47C7-BDA8-FBE366399D2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{54E0EE64-5DA5-47C7-BDA8-FBE366399D2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -108,22 +108,28 @@
     <t>LSTM, Write Evaluation, put figures in, check what to change in figures, create all chapter outlines and write rought summary for all of them</t>
   </si>
   <si>
-    <t>LSTM, Clean up evaluation/generate missing plots, identify what theory is needed to explain evaluation, write theory</t>
-  </si>
-  <si>
-    <t>LSTM, Write most of theory, LSTM, metrics/loss function</t>
-  </si>
-  <si>
     <t>LSTM, Write creation of datasets, odes, normalization</t>
   </si>
   <si>
     <t>LSTM, Write training theory, hyperparameter overview, hyperparameter search manually vs autotuner</t>
   </si>
   <si>
-    <t>LSTM, Write other work chapter, introduction</t>
-  </si>
-  <si>
     <t>LSTM, Clean up writing, check for things that need more work, make new plan for rest</t>
+  </si>
+  <si>
+    <t>LSTM, Clean up evaluation/generate missing plots, identify what methods are needed to explain evaluation, write methods</t>
+  </si>
+  <si>
+    <t>LSTM, Write most of methods, LSTM, metrics/loss function</t>
+  </si>
+  <si>
+    <t>LSTM, Write "other work" chapter, introduction</t>
+  </si>
+  <si>
+    <t>Abgabe fast fertig</t>
+  </si>
+  <si>
+    <t>Abgabe final</t>
   </si>
 </sst>
 </file>
@@ -476,16 +482,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C820AA12-46EE-47CA-80CD-C145E0B71ADB}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="121.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="127.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -639,9 +645,6 @@
         <f t="array" ref="B13">_xlfn.SWITCH(WEEKDAY(A13,1),1,"Sun",2,"Mon",3,"Tue",4,"Wed",5,"Thu",6,"Fri",7,"Sat")</f>
         <v>Wed</v>
       </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -652,7 +655,7 @@
         <v>Thu</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -664,7 +667,7 @@
         <v>Fri</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -676,7 +679,7 @@
         <v>Sat</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -688,7 +691,7 @@
         <v>Sun</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -700,7 +703,7 @@
         <v>Mon</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -712,7 +715,7 @@
         <v>Tue</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -735,6 +738,9 @@
         <f t="array" ref="B21">_xlfn.SWITCH(WEEKDAY(A21,1),1,"Sun",2,"Mon",3,"Tue",4,"Wed",5,"Thu",6,"Fri",7,"Sat")</f>
         <v>Thu</v>
       </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -788,6 +794,93 @@
       <c r="B27" t="str" cm="1">
         <f t="array" ref="B27">_xlfn.SWITCH(WEEKDAY(A27,1),1,"Sun",2,"Mon",3,"Tue",4,"Wed",5,"Thu",6,"Fri",7,"Sat")</f>
         <v>Wed</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>44896</v>
+      </c>
+      <c r="B28" t="str" cm="1">
+        <f t="array" ref="B28">_xlfn.SWITCH(WEEKDAY(A28,1),1,"Sun",2,"Mon",3,"Tue",4,"Wed",5,"Thu",6,"Fri",7,"Sat")</f>
+        <v>Thu</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>44897</v>
+      </c>
+      <c r="B29" t="str" cm="1">
+        <f t="array" ref="B29">_xlfn.SWITCH(WEEKDAY(A29,1),1,"Sun",2,"Mon",3,"Tue",4,"Wed",5,"Thu",6,"Fri",7,"Sat")</f>
+        <v>Fri</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>44898</v>
+      </c>
+      <c r="B30" t="str" cm="1">
+        <f t="array" ref="B30">_xlfn.SWITCH(WEEKDAY(A30,1),1,"Sun",2,"Mon",3,"Tue",4,"Wed",5,"Thu",6,"Fri",7,"Sat")</f>
+        <v>Sat</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>44899</v>
+      </c>
+      <c r="B31" t="str" cm="1">
+        <f t="array" ref="B31">_xlfn.SWITCH(WEEKDAY(A31,1),1,"Sun",2,"Mon",3,"Tue",4,"Wed",5,"Thu",6,"Fri",7,"Sat")</f>
+        <v>Sun</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>44900</v>
+      </c>
+      <c r="B32" t="str" cm="1">
+        <f t="array" ref="B32">_xlfn.SWITCH(WEEKDAY(A32,1),1,"Sun",2,"Mon",3,"Tue",4,"Wed",5,"Thu",6,"Fri",7,"Sat")</f>
+        <v>Mon</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>44901</v>
+      </c>
+      <c r="B33" t="str" cm="1">
+        <f t="array" ref="B33">_xlfn.SWITCH(WEEKDAY(A33,1),1,"Sun",2,"Mon",3,"Tue",4,"Wed",5,"Thu",6,"Fri",7,"Sat")</f>
+        <v>Tue</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>44902</v>
+      </c>
+      <c r="B34" t="str" cm="1">
+        <f t="array" ref="B34">_xlfn.SWITCH(WEEKDAY(A34,1),1,"Sun",2,"Mon",3,"Tue",4,"Wed",5,"Thu",6,"Fri",7,"Sat")</f>
+        <v>Wed</v>
+      </c>
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>44903</v>
+      </c>
+      <c r="B35" t="str" cm="1">
+        <f t="array" ref="B35">_xlfn.SWITCH(WEEKDAY(A35,1),1,"Sun",2,"Mon",3,"Tue",4,"Wed",5,"Thu",6,"Fri",7,"Sat")</f>
+        <v>Thu</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>44904</v>
+      </c>
+      <c r="B36" t="str" cm="1">
+        <f t="array" ref="B36">_xlfn.SWITCH(WEEKDAY(A36,1),1,"Sun",2,"Mon",3,"Tue",4,"Wed",5,"Thu",6,"Fri",7,"Sat")</f>
+        <v>Fri</v>
       </c>
     </row>
   </sheetData>

</xml_diff>